<commit_message>
Tweaks, try out 50% diagram size
</commit_message>
<xml_diff>
--- a/other/plot_data.xlsx
+++ b/other/plot_data.xlsx
@@ -262,11 +262,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68160128"/>
-        <c:axId val="68158592"/>
+        <c:axId val="146219392"/>
+        <c:axId val="146221696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68160128"/>
+        <c:axId val="146219392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,12 +300,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68158592"/>
+        <c:crossAx val="146221696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68158592"/>
+        <c:axId val="146221696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -317,16 +317,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68160128"/>
+        <c:crossAx val="146219392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -505,11 +500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68415872"/>
-        <c:axId val="68417408"/>
+        <c:axId val="146254080"/>
+        <c:axId val="146285312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68415872"/>
+        <c:axId val="146254080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,12 +533,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68417408"/>
+        <c:crossAx val="146285312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68417408"/>
+        <c:axId val="146285312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -555,16 +550,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68415872"/>
+        <c:crossAx val="146254080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -933,7 +923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>